<commit_message>
update due to suppressing oids
</commit_message>
<xml_diff>
--- a/CodeSystem-Hn-AppointmentTypeProposed-New-Codes-cs.xlsx
+++ b/CodeSystem-Hn-AppointmentTypeProposed-New-Codes-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -54,10 +54,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-05T16:09:33+02:00</t>
+    <t>2023-10-09T22:41:16+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -340,102 +343,104 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -453,75 +458,75 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2"/>
     </row>

</xml_diff>

<commit_message>
update - due to fix off app-4 error on no-basis-appointment
</commit_message>
<xml_diff>
--- a/CodeSystem-Hn-AppointmentTypeProposed-New-Codes-cs.xlsx
+++ b/CodeSystem-Hn-AppointmentTypeProposed-New-Codes-cs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.9.0</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-15T12:00:41+01:00</t>
+    <t>2025-06-05T14:31:57+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>